<commit_message>
backup class calculation v2
</commit_message>
<xml_diff>
--- a/public/jerman_A.xlsx
+++ b/public/jerman_A.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
   <si>
     <t>jerman_A</t>
   </si>
@@ -26,25 +26,100 @@
     <t>Nama Siswa</t>
   </si>
   <si>
+    <t>X MIPA 2</t>
+  </si>
+  <si>
+    <t>DEFI SETIYOWATI</t>
+  </si>
+  <si>
+    <t>X MIPA 6</t>
+  </si>
+  <si>
+    <t>LUKE ARINDA FEBRYOLA</t>
+  </si>
+  <si>
+    <t>NADIA RAHMA WINDARINI</t>
+  </si>
+  <si>
     <t>X MIPA 1</t>
   </si>
   <si>
+    <t>EVI BUDI APRIYANI</t>
+  </si>
+  <si>
+    <t>LINDA SRI LESTARI</t>
+  </si>
+  <si>
+    <t>ALFIRA SELFIANA PUTRI</t>
+  </si>
+  <si>
+    <t>POPPY TRI UTAMI</t>
+  </si>
+  <si>
+    <t>X MIPA 4</t>
+  </si>
+  <si>
+    <t>FAUZAN BILAL MAHARDIKA</t>
+  </si>
+  <si>
+    <t>RICO HENDRIAWAN</t>
+  </si>
+  <si>
+    <t>LALA ERLINDA</t>
+  </si>
+  <si>
     <t>ANDIKA IRDI  PERMANA</t>
   </si>
   <si>
-    <t>EVI BUDI APRIYANI</t>
-  </si>
-  <si>
-    <t>LINDA SRI LESTARI</t>
-  </si>
-  <si>
-    <t>X MIPA 2</t>
-  </si>
-  <si>
-    <t>ALFIRA SELFIANA PUTRI</t>
-  </si>
-  <si>
-    <t>DEFI SETIYOWATI</t>
+    <t>X MIPA 5</t>
+  </si>
+  <si>
+    <t>ALINSYA NICO OVIYANA</t>
+  </si>
+  <si>
+    <t>ADELLIA HANDAYANI</t>
+  </si>
+  <si>
+    <t>X MIPA 3</t>
+  </si>
+  <si>
+    <t>DHIMAS YUDIYATMOKO</t>
+  </si>
+  <si>
+    <t>EKA PANJI SATRIA</t>
+  </si>
+  <si>
+    <t>GEISKA AYU WULAN ANGGRAENY</t>
+  </si>
+  <si>
+    <t>INTAN MUSTIKA SARI</t>
+  </si>
+  <si>
+    <t>PUJI LESTARI</t>
+  </si>
+  <si>
+    <t>RIZKY ADI NUGROHO</t>
+  </si>
+  <si>
+    <t>ANNISA DHEKA CAHYANINGTYAS</t>
+  </si>
+  <si>
+    <t>GERA DWIDYA AYU SHELYMAR</t>
+  </si>
+  <si>
+    <t>SYIFA AMANDA PUTRI</t>
+  </si>
+  <si>
+    <t>APNAMIRA DWI NOOR RIYANTI</t>
+  </si>
+  <si>
+    <t>AMELIANA PUTRI</t>
+  </si>
+  <si>
+    <t>YOVI SAPUTRA</t>
+  </si>
+  <si>
+    <t>FARIDA DWI LESTARI</t>
   </si>
   <si>
     <t>INDRA SETIAWAN</t>
@@ -53,88 +128,28 @@
     <t>MOHAMAD TOUFIK HIDAYAT</t>
   </si>
   <si>
-    <t>POPPY TRI UTAMI</t>
-  </si>
-  <si>
-    <t>X MIPA 3</t>
-  </si>
-  <si>
-    <t>AMELIANA PUTRI</t>
-  </si>
-  <si>
-    <t>APNAMIRA DWI NOOR RIYANTI</t>
-  </si>
-  <si>
-    <t>DHIMAS YUDIYATMOKO</t>
-  </si>
-  <si>
-    <t>EKA PANJI SATRIA</t>
-  </si>
-  <si>
-    <t>GEISKA AYU WULAN ANGGRAENY</t>
-  </si>
-  <si>
-    <t>INTAN MUSTIKA SARI</t>
-  </si>
-  <si>
-    <t>SYIFA AMANDA PUTRI</t>
-  </si>
-  <si>
-    <t>X MIPA 4</t>
-  </si>
-  <si>
-    <t>FAUZAN BILAL MAHARDIKA</t>
-  </si>
-  <si>
-    <t>PUJI LESTARI</t>
-  </si>
-  <si>
-    <t>RICO HENDRIAWAN</t>
-  </si>
-  <si>
-    <t>X MIPA 5</t>
-  </si>
-  <si>
-    <t>ALINSYA NICO OVIYANA</t>
-  </si>
-  <si>
-    <t>FARIDA DWI LESTARI</t>
-  </si>
-  <si>
-    <t>GERA DWIDYA AYU SHELYMAR</t>
-  </si>
-  <si>
-    <t>X MIPA 6</t>
-  </si>
-  <si>
-    <t>ADELLIA HANDAYANI</t>
-  </si>
-  <si>
-    <t>ANNISA DHEKA CAHYANINGTYAS</t>
-  </si>
-  <si>
-    <t>LALA ERLINDA</t>
-  </si>
-  <si>
-    <t>LUKE ARINDA FEBRYOLA</t>
-  </si>
-  <si>
-    <t>NADIA RAHMA WINDARINI</t>
-  </si>
-  <si>
-    <t>RIZKY ADI NUGROHO</t>
-  </si>
-  <si>
-    <t>YOVI SAPUTRA</t>
-  </si>
-  <si>
     <t>FAJAR QOMARUDIN</t>
   </si>
   <si>
-    <t>GALANG EKA KURNIAWAN</t>
-  </si>
-  <si>
-    <t>SEBTIE MEGA ANGGRAINI</t>
+    <t>SEPTA AL AKBAR</t>
+  </si>
+  <si>
+    <t>RENDITYA HIKMAL ARYANTARA</t>
+  </si>
+  <si>
+    <t>NAJWA ANJELIA RAHMA TANTIA</t>
+  </si>
+  <si>
+    <t>FABIZAN ARKIANTO</t>
+  </si>
+  <si>
+    <t>DITO OKTA SETYAWAN</t>
+  </si>
+  <si>
+    <t>KEVIN NUR SO'IM</t>
+  </si>
+  <si>
+    <t>DIA AYU LESTARI</t>
   </si>
 </sst>
 </file>
@@ -473,7 +488,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,58 +519,58 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -563,55 +578,55 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -619,7 +634,7 @@
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -627,44 +642,44 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
         <v>30</v>
@@ -672,7 +687,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
         <v>31</v>
@@ -680,7 +695,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
         <v>32</v>
@@ -688,7 +703,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
         <v>33</v>
@@ -696,7 +711,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B28" t="s">
         <v>34</v>
@@ -704,7 +719,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="B29" t="s">
         <v>35</v>
@@ -712,7 +727,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="B30" t="s">
         <v>36</v>
@@ -720,7 +735,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B31" t="s">
         <v>37</v>
@@ -728,7 +743,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B32" t="s">
         <v>38</v>
@@ -736,10 +751,50 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>